<commit_message>
Added main.py and front end
</commit_message>
<xml_diff>
--- a/data/video/exportvideo.xlsx
+++ b/data/video/exportvideo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,7 +456,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>angry</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -606,7 +606,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -616,7 +616,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -646,7 +646,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>angry</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>happy</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -766,7 +766,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>angry</t>
+          <t>neutral</t>
         </is>
       </c>
     </row>
@@ -775,6 +775,336 @@
         <v>33</v>
       </c>
       <c r="B35" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="inlineStr">
         <is>
           <t>neutral</t>
         </is>

</xml_diff>